<commit_message>
adding standard curve information
</commit_message>
<xml_diff>
--- a/docs/eDNA qPCR/example output/Results.xlsx
+++ b/docs/eDNA qPCR/example output/Results.xlsx
@@ -880,10 +880,10 @@
         <v>5</v>
       </c>
       <c r="R9">
-        <v>1.833294966598223</v>
+        <v>1.870901181057595</v>
       </c>
       <c r="S9">
-        <v>0.4522917900861022</v>
+        <v>0.4580182439559286</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -1060,10 +1060,10 @@
         <v>6</v>
       </c>
       <c r="R12">
-        <v>56.84180167885265</v>
+        <v>57.58568459491445</v>
       </c>
       <c r="S12">
-        <v>1.762241812069973</v>
+        <v>1.767791509175992</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
@@ -1130,10 +1130,10 @@
         <v>1</v>
       </c>
       <c r="R13">
-        <v>1.025595968520667</v>
+        <v>1.047927592285356</v>
       </c>
       <c r="S13">
-        <v>0.3065528239756051</v>
+        <v>0.3113145974078815</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
@@ -1200,10 +1200,10 @@
         <v>6</v>
       </c>
       <c r="R14">
-        <v>8.47381742825816</v>
+        <v>8.632235739018183</v>
       </c>
       <c r="S14">
-        <v>0.9765250111008219</v>
+        <v>0.9837271029525712</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>6</v>
       </c>
       <c r="R15">
-        <v>54.06053278856787</v>
+        <v>54.77386105131029</v>
       </c>
       <c r="S15">
-        <v>1.740840409491302</v>
+        <v>1.746430710391437</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -1340,10 +1340,10 @@
         <v>6</v>
       </c>
       <c r="R16">
-        <v>469.1353020052179</v>
+        <v>473.1462862645127</v>
       </c>
       <c r="S16">
-        <v>2.672222863165362</v>
+        <v>2.675912353311067</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
@@ -1410,10 +1410,10 @@
         <v>6</v>
       </c>
       <c r="R17">
-        <v>969.244766861823</v>
+        <v>976.0242192382194</v>
       </c>
       <c r="S17">
-        <v>2.986881308996013</v>
+        <v>2.989905329482484</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
@@ -1523,10 +1523,10 @@
         <v>5</v>
       </c>
       <c r="R19">
-        <v>46.11392850618222</v>
+        <v>46.73820180873648</v>
       </c>
       <c r="S19">
-        <v>1.673149318575401</v>
+        <v>1.678866056077288</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
@@ -1593,10 +1593,10 @@
         <v>6</v>
       </c>
       <c r="R20">
-        <v>313.1837250105402</v>
+        <v>316.1329298790346</v>
       </c>
       <c r="S20">
-        <v>2.497183684455768</v>
+        <v>2.501241339858165</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
@@ -1663,10 +1663,10 @@
         <v>3</v>
       </c>
       <c r="R21">
-        <v>1.411958576851275</v>
+        <v>1.441722400822429</v>
       </c>
       <c r="S21">
-        <v>0.3823698449277351</v>
+        <v>0.3876962875187916</v>
       </c>
       <c r="T21" t="inlineStr">
         <is>
@@ -1733,10 +1733,10 @@
         <v>6</v>
       </c>
       <c r="R22">
-        <v>3.557827998537906</v>
+        <v>3.625693341108359</v>
       </c>
       <c r="S22">
-        <v>0.6587579319248011</v>
+        <v>0.6651768379722269</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
@@ -1803,10 +1803,10 @@
         <v>6</v>
       </c>
       <c r="R23">
-        <v>1.598660175325356</v>
+        <v>1.63192857169589</v>
       </c>
       <c r="S23">
-        <v>0.414749490878346</v>
+        <v>0.4202740987187935</v>
       </c>
       <c r="T23" t="inlineStr">
         <is>
@@ -1873,10 +1873,10 @@
         <v>6</v>
       </c>
       <c r="R24">
-        <v>128.6627375096496</v>
+        <v>130.120275196242</v>
       </c>
       <c r="S24">
-        <v>2.112815186423022</v>
+        <v>2.117669852063998</v>
       </c>
       <c r="T24" t="inlineStr">
         <is>
@@ -1943,10 +1943,10 @@
         <v>6</v>
       </c>
       <c r="R25">
-        <v>43.33866190069224</v>
+        <v>43.931163323227</v>
       </c>
       <c r="S25">
-        <v>1.646782582375346</v>
+        <v>1.652547663158297</v>
       </c>
       <c r="T25" t="inlineStr">
         <is>
@@ -2013,10 +2013,10 @@
         <v>6</v>
       </c>
       <c r="R26">
-        <v>78.68553352397679</v>
+        <v>79.66017359891231</v>
       </c>
       <c r="S26">
-        <v>1.901379484746539</v>
+        <v>1.906659152372425</v>
       </c>
       <c r="T26" t="inlineStr">
         <is>
@@ -2144,10 +2144,10 @@
         <v>3</v>
       </c>
       <c r="R28">
-        <v>3.090498661548979</v>
+        <v>3.150393046867427</v>
       </c>
       <c r="S28">
-        <v>0.6117762548919481</v>
+        <v>0.6180892268332367</v>
       </c>
       <c r="T28" t="inlineStr">
         <is>
@@ -2214,10 +2214,10 @@
         <v>6</v>
       </c>
       <c r="R29">
-        <v>27.75203441798526</v>
+        <v>28.158123859662</v>
       </c>
       <c r="S29">
-        <v>1.458668579642894</v>
+        <v>1.464759576449468</v>
       </c>
       <c r="T29" t="inlineStr">
         <is>
@@ -2284,10 +2284,10 @@
         <v>3</v>
       </c>
       <c r="R30">
-        <v>0.9050636616932157</v>
+        <v>0.9250166959981613</v>
       </c>
       <c r="S30">
-        <v>0.2799094931140583</v>
+        <v>0.2844345005709749</v>
       </c>
       <c r="T30" t="inlineStr">
         <is>
@@ -2354,10 +2354,10 @@
         <v>6</v>
       </c>
       <c r="R31">
-        <v>1.856847185659114</v>
+        <v>1.89488508297257</v>
       </c>
       <c r="S31">
-        <v>0.4558870103512557</v>
+        <v>0.4616313284014649</v>
       </c>
       <c r="T31" t="inlineStr">
         <is>
@@ -2424,10 +2424,10 @@
         <v>2</v>
       </c>
       <c r="R32">
-        <v>1.624434045617239</v>
+        <v>1.658182399630851</v>
       </c>
       <c r="S32">
-        <v>0.4190356630312285</v>
+        <v>0.4245847781248915</v>
       </c>
       <c r="T32" t="inlineStr">
         <is>
@@ -2494,10 +2494,10 @@
         <v>3</v>
       </c>
       <c r="R33">
-        <v>2.375628634453482</v>
+        <v>2.423023938719238</v>
       </c>
       <c r="S33">
-        <v>0.5283546622193416</v>
+        <v>0.5344099363617495</v>
       </c>
       <c r="T33" t="inlineStr">
         <is>
@@ -2564,10 +2564,10 @@
         <v>2</v>
       </c>
       <c r="R34">
-        <v>0.5284580866581514</v>
+        <v>0.5407268426004352</v>
       </c>
       <c r="S34">
-        <v>0.1842535340122822</v>
+        <v>0.1877256489281545</v>
       </c>
       <c r="T34" t="inlineStr">
         <is>
@@ -2634,10 +2634,10 @@
         <v>1</v>
       </c>
       <c r="R35">
-        <v>1.239819879647664</v>
+        <v>1.26630512812856</v>
       </c>
       <c r="S35">
-        <v>0.3502130949322217</v>
+        <v>0.3553183814944465</v>
       </c>
       <c r="T35" t="inlineStr">
         <is>
@@ -2704,10 +2704,10 @@
         <v>4</v>
       </c>
       <c r="R36">
-        <v>3.153764759510794</v>
+        <v>3.214746706901876</v>
       </c>
       <c r="S36">
-        <v>0.6184418974616588</v>
+        <v>0.6247714800046056</v>
       </c>
       <c r="T36" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>4</v>
       </c>
       <c r="R37">
-        <v>3.813053986049853</v>
+        <v>3.885215271104165</v>
       </c>
       <c r="S37">
-        <v>0.6824207330075184</v>
+        <v>0.6888837060266939</v>
       </c>
       <c r="T37" t="inlineStr">
         <is>
@@ -2844,10 +2844,10 @@
         <v>5</v>
       </c>
       <c r="R38">
-        <v>1.731460539847939</v>
+        <v>1.767192603285276</v>
       </c>
       <c r="S38">
-        <v>0.4363949308436154</v>
+        <v>0.4420393881373103</v>
       </c>
       <c r="T38" t="inlineStr">
         <is>
@@ -2914,10 +2914,10 @@
         <v>1</v>
       </c>
       <c r="R39">
-        <v>0.8668793656929291</v>
+        <v>0.886071812742895</v>
       </c>
       <c r="S39">
-        <v>0.2711162555459977</v>
+        <v>0.2755582246071517</v>
       </c>
       <c r="T39" t="inlineStr">
         <is>
@@ -2984,10 +2984,10 @@
         <v>6</v>
       </c>
       <c r="R40">
-        <v>9.365324036842338</v>
+        <v>9.524342519382833</v>
       </c>
       <c r="S40">
-        <v>1.015582883392046</v>
+        <v>1.022194973949702</v>
       </c>
       <c r="T40" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>6</v>
       </c>
       <c r="R42">
-        <v>1.960175122500279</v>
+        <v>2.0000993536122</v>
       </c>
       <c r="S42">
-        <v>0.4713174044663047</v>
+        <v>0.4771356373900139</v>
       </c>
       <c r="T42" t="inlineStr">
         <is>
@@ -3185,10 +3185,10 @@
         <v>1</v>
       </c>
       <c r="R43">
-        <v>0.8067362009614096</v>
+        <v>0.8247231992570295</v>
       </c>
       <c r="S43">
-        <v>0.2568947464567651</v>
+        <v>0.2611969936403649</v>
       </c>
       <c r="T43" t="inlineStr">
         <is>
@@ -3255,10 +3255,10 @@
         <v>6</v>
       </c>
       <c r="R44">
-        <v>3.645584590354808</v>
+        <v>3.714931372753841</v>
       </c>
       <c r="S44">
-        <v>0.6670403724503207</v>
+        <v>0.6734753758323673</v>
       </c>
       <c r="T44" t="inlineStr">
         <is>
@@ -3508,10 +3508,10 @@
         <v>1</v>
       </c>
       <c r="R48">
-        <v>0.5493288301136972</v>
+        <v>0.5620358249665113</v>
       </c>
       <c r="S48">
-        <v>0.1901436023607954</v>
+        <v>0.1936909901090488</v>
       </c>
       <c r="T48" t="inlineStr">
         <is>
@@ -3944,10 +3944,10 @@
         <v>1</v>
       </c>
       <c r="R55">
-        <v>0.5066191978776918</v>
+        <v>0.5184274680391626</v>
       </c>
       <c r="S55">
-        <v>0.1780034970665818</v>
+        <v>0.1813940514517223</v>
       </c>
       <c r="T55" t="inlineStr">
         <is>
@@ -4075,10 +4075,10 @@
         <v>1</v>
       </c>
       <c r="R57">
-        <v>1.226395609895802</v>
+        <v>1.252623087665084</v>
       </c>
       <c r="S57">
-        <v>0.3476023369659849</v>
+        <v>0.3526885309866088</v>
       </c>
       <c r="T57" t="inlineStr">
         <is>
@@ -4145,10 +4145,10 @@
         <v>1</v>
       </c>
       <c r="R58">
-        <v>3.102399901721531</v>
+        <v>3.165109855994819</v>
       </c>
       <c r="S58">
-        <v>0.6130379930986004</v>
+        <v>0.6196264605382849</v>
       </c>
       <c r="T58" t="inlineStr">
         <is>
@@ -4398,10 +4398,10 @@
         <v>2</v>
       </c>
       <c r="R62">
-        <v>0.3176184063310598</v>
+        <v>0.3253443451059597</v>
       </c>
       <c r="S62">
-        <v>0.1197896530349349</v>
+        <v>0.1223287294051758</v>
       </c>
       <c r="T62" t="inlineStr">
         <is>
@@ -5261,10 +5261,10 @@
         <v>2</v>
       </c>
       <c r="R76">
-        <v>0.693516480208653</v>
+        <v>0.7092071748480213</v>
       </c>
       <c r="S76">
-        <v>0.2287894272746282</v>
+        <v>0.2327947072146441</v>
       </c>
       <c r="T76" t="inlineStr">
         <is>
@@ -5819,10 +5819,10 @@
         <v>6</v>
       </c>
       <c r="R85">
-        <v>8.534270336700185</v>
+        <v>8.680893291705946</v>
       </c>
       <c r="S85">
-        <v>0.9792874618424032</v>
+        <v>0.9859154331099647</v>
       </c>
       <c r="T85" t="inlineStr">
         <is>
@@ -6957,10 +6957,10 @@
         <v>6</v>
       </c>
       <c r="R104">
-        <v>11.5047155212516</v>
+        <v>11.70653431521832</v>
       </c>
       <c r="S104">
-        <v>1.097073816102029</v>
+        <v>1.104027113652473</v>
       </c>
       <c r="T104" t="inlineStr">
         <is>
@@ -7149,10 +7149,10 @@
         <v>5</v>
       </c>
       <c r="R107">
-        <v>0.6949691382259547</v>
+        <v>0.7106895364787947</v>
       </c>
       <c r="S107">
-        <v>0.2291617950345642</v>
+        <v>0.2331711990043615</v>
       </c>
       <c r="T107" t="inlineStr">
         <is>
@@ -7463,10 +7463,10 @@
         <v>1</v>
       </c>
       <c r="R112">
-        <v>1.360505772799696</v>
+        <v>1.389294654818555</v>
       </c>
       <c r="S112">
-        <v>0.3730050668693654</v>
+        <v>0.3782697115208322</v>
       </c>
       <c r="T112" t="inlineStr">
         <is>
@@ -7777,10 +7777,10 @@
         <v>1</v>
       </c>
       <c r="R117">
-        <v>0.3992069295834126</v>
+        <v>0.4087187001793404</v>
       </c>
       <c r="S117">
-        <v>0.1458819473228112</v>
+        <v>0.1488242797264549</v>
       </c>
       <c r="T117" t="inlineStr">
         <is>
@@ -7847,10 +7847,10 @@
         <v>1</v>
       </c>
       <c r="R118">
-        <v>0.545580835243035</v>
+        <v>0.5582092593561443</v>
       </c>
       <c r="S118">
-        <v>0.1890917239783804</v>
+        <v>0.1926257807312954</v>
       </c>
       <c r="T118" t="inlineStr">
         <is>
@@ -8039,10 +8039,10 @@
         <v>2</v>
       </c>
       <c r="R121">
-        <v>0.9154404116246164</v>
+        <v>0.9355995287148497</v>
       </c>
       <c r="S121">
-        <v>0.2822686458491669</v>
+        <v>0.2868155076933723</v>
       </c>
       <c r="T121" t="inlineStr">
         <is>
@@ -8114,10 +8114,10 @@
         <v>6</v>
       </c>
       <c r="R122">
-        <v>45.9529594561365</v>
+        <v>46.59038322156842</v>
       </c>
       <c r="S122">
-        <v>1.671662971148734</v>
+        <v>1.677519201969222</v>
       </c>
       <c r="T122" t="inlineStr">
         <is>
@@ -8189,10 +8189,10 @@
         <v>5</v>
       </c>
       <c r="R123">
-        <v>1.1591156592586</v>
+        <v>1.185641823985728</v>
       </c>
       <c r="S123">
-        <v>0.3342759071940755</v>
+        <v>0.3395789926495084</v>
       </c>
       <c r="T123" t="inlineStr">
         <is>
@@ -8264,10 +8264,10 @@
         <v>4</v>
       </c>
       <c r="R124">
-        <v>7.300488355497967</v>
+        <v>7.439323364126635</v>
       </c>
       <c r="S124">
-        <v>0.9191036446482111</v>
+        <v>0.9263076277860751</v>
       </c>
       <c r="T124" t="inlineStr">
         <is>
@@ -8453,10 +8453,10 @@
         <v>1</v>
       </c>
       <c r="R127">
-        <v>2.82287662287342</v>
+        <v>2.882365397774951</v>
       </c>
       <c r="S127">
-        <v>0.5823902820970053</v>
+        <v>0.5890964076029308</v>
       </c>
       <c r="T127" t="inlineStr">
         <is>
@@ -8528,10 +8528,10 @@
         <v>3</v>
       </c>
       <c r="R128">
-        <v>3.413070443884553</v>
+        <v>3.478481813310682</v>
       </c>
       <c r="S128">
-        <v>0.6447408599525561</v>
+        <v>0.6511308149254167</v>
       </c>
       <c r="T128" t="inlineStr">
         <is>
@@ -8603,10 +8603,10 @@
         <v>2</v>
       </c>
       <c r="R129">
-        <v>2.90075697323957</v>
+        <v>2.957372605549809</v>
       </c>
       <c r="S129">
-        <v>0.5911488935394756</v>
+        <v>0.5974069430928867</v>
       </c>
       <c r="T129" t="inlineStr">
         <is>
@@ -8678,10 +8678,10 @@
         <v>6</v>
       </c>
       <c r="R130">
-        <v>21.7344597342841</v>
+        <v>22.09593464075914</v>
       </c>
       <c r="S130">
-        <v>1.356684638012994</v>
+        <v>1.363535541863407</v>
       </c>
       <c r="T130" t="inlineStr">
         <is>
@@ -8753,10 +8753,10 @@
         <v>6</v>
       </c>
       <c r="R131">
-        <v>16.30798246348245</v>
+        <v>16.58962251844254</v>
       </c>
       <c r="S131">
-        <v>1.238246446497991</v>
+        <v>1.245256519393987</v>
       </c>
       <c r="T131" t="inlineStr">
         <is>
@@ -8894,10 +8894,10 @@
         <v>1</v>
       </c>
       <c r="R133">
-        <v>0.3614949607831182</v>
+        <v>0.3701862945602766</v>
       </c>
       <c r="S133">
-        <v>0.1340160382517197</v>
+        <v>0.1367796191265753</v>
       </c>
       <c r="T133" t="inlineStr">
         <is>
@@ -9233,10 +9233,10 @@
         <v>3</v>
       </c>
       <c r="R138">
-        <v>1.742300570958643</v>
+        <v>1.780848398445973</v>
       </c>
       <c r="S138">
-        <v>0.4381150540839663</v>
+        <v>0.4441773133830383</v>
       </c>
       <c r="T138" t="inlineStr">
         <is>
@@ -9308,10 +9308,10 @@
         <v>6</v>
       </c>
       <c r="R139">
-        <v>2.391083620188534</v>
+        <v>2.442220573432152</v>
       </c>
       <c r="S139">
-        <v>0.5303384991082838</v>
+        <v>0.5368386959610926</v>
       </c>
       <c r="T139" t="inlineStr">
         <is>
@@ -9383,10 +9383,10 @@
         <v>4</v>
       </c>
       <c r="R140">
-        <v>2.585682922971238</v>
+        <v>2.640682812932694</v>
       </c>
       <c r="S140">
-        <v>0.5545718828579896</v>
+        <v>0.5611828435608059</v>
       </c>
       <c r="T140" t="inlineStr">
         <is>
@@ -9514,10 +9514,10 @@
         <v>6</v>
       </c>
       <c r="R143">
-        <v>47.08614491562275</v>
+        <v>47.72146225222763</v>
       </c>
       <c r="S143">
-        <v>1.682019960916959</v>
+        <v>1.687720314077689</v>
       </c>
       <c r="T143" t="inlineStr">
         <is>
@@ -9635,10 +9635,10 @@
         <v>2</v>
       </c>
       <c r="R147">
-        <v>1.0739170093528</v>
+        <v>1.097193358193166</v>
       </c>
       <c r="S147">
-        <v>0.3167913735085373</v>
+        <v>0.3216384736341777</v>
       </c>
       <c r="T147" t="inlineStr">
         <is>
@@ -9672,10 +9672,10 @@
         <v>4</v>
       </c>
       <c r="R148">
-        <v>2.250014060724717</v>
+        <v>2.295168426947501</v>
       </c>
       <c r="S148">
-        <v>0.5118852398963964</v>
+        <v>0.5178776177234982</v>
       </c>
       <c r="T148" t="inlineStr">
         <is>
@@ -9709,10 +9709,10 @@
         <v>6</v>
       </c>
       <c r="R149">
-        <v>34.7340041191838</v>
+        <v>35.26361622431453</v>
       </c>
       <c r="S149">
-        <v>1.553081683133146</v>
+        <v>1.559471109962378</v>
       </c>
       <c r="T149" t="inlineStr">
         <is>
@@ -9746,10 +9746,10 @@
         <v>1</v>
       </c>
       <c r="R150">
-        <v>3.236780136799685</v>
+        <v>3.299184985570151</v>
       </c>
       <c r="S150">
-        <v>0.627035927335381</v>
+        <v>0.6333861323661171</v>
       </c>
       <c r="T150" t="inlineStr">
         <is>
@@ -9839,10 +9839,10 @@
         <v>1</v>
       </c>
       <c r="R153">
-        <v>1.278435762843094</v>
+        <v>1.305660762531532</v>
       </c>
       <c r="S153">
-        <v>0.3576367887946829</v>
+        <v>0.3627954088569834</v>
       </c>
       <c r="T153" t="inlineStr">
         <is>
@@ -9876,10 +9876,10 @@
         <v>1</v>
       </c>
       <c r="R154">
-        <v>3.529888270118433</v>
+        <v>3.597280978501602</v>
       </c>
       <c r="S154">
-        <v>0.656087490253573</v>
+        <v>0.6625010479494922</v>
       </c>
       <c r="T154" t="inlineStr">
         <is>
@@ -9913,10 +9913,10 @@
         <v>6</v>
       </c>
       <c r="R155">
-        <v>15.62495315579372</v>
+        <v>15.87296903244873</v>
       </c>
       <c r="S155">
-        <v>1.220760430263325</v>
+        <v>1.227191509438888</v>
       </c>
       <c r="T155" t="inlineStr">
         <is>
@@ -10006,10 +10006,10 @@
         <v>1</v>
       </c>
       <c r="R158">
-        <v>0.4551408859244814</v>
+        <v>0.4658554472824853</v>
       </c>
       <c r="S158">
-        <v>0.1629050435057669</v>
+        <v>0.1660911452417727</v>
       </c>
       <c r="T158" t="inlineStr">
         <is>
@@ -10127,10 +10127,10 @@
         <v>5</v>
       </c>
       <c r="R162">
-        <v>1.677986790035256</v>
+        <v>1.712729579514816</v>
       </c>
       <c r="S162">
-        <v>0.427808430394831</v>
+        <v>0.4334065029477489</v>
       </c>
       <c r="T162" t="inlineStr">
         <is>
@@ -10248,10 +10248,10 @@
         <v>1</v>
       </c>
       <c r="R166">
-        <v>0.8495016651154873</v>
+        <v>0.8683467697500011</v>
       </c>
       <c r="S166">
-        <v>0.2670547266490567</v>
+        <v>0.2714574854980195</v>
       </c>
       <c r="T166" t="inlineStr">
         <is>
@@ -10313,10 +10313,10 @@
         <v>2</v>
       </c>
       <c r="R168">
-        <v>2.327454350730597</v>
+        <v>2.373991978051463</v>
       </c>
       <c r="S168">
-        <v>0.5221121061116129</v>
+        <v>0.5281440456828261</v>
       </c>
       <c r="T168" t="inlineStr">
         <is>
@@ -10378,10 +10378,10 @@
         <v>1</v>
       </c>
       <c r="R170">
-        <v>0.7260197355232731</v>
+        <v>0.7423734953297659</v>
       </c>
       <c r="S170">
-        <v>0.2370457571844363</v>
+        <v>0.2411412560528974</v>
       </c>
       <c r="T170" t="inlineStr">
         <is>
@@ -10443,10 +10443,10 @@
         <v>6</v>
       </c>
       <c r="R172">
-        <v>18.97324833598926</v>
+        <v>19.2664548137769</v>
       </c>
       <c r="S172">
-        <v>1.300448701809729</v>
+        <v>1.306777784732914</v>
       </c>
       <c r="T172" t="inlineStr">
         <is>

</xml_diff>